<commit_message>
aCoComparacion IBC, Inflación, Bitcoin, Dólar
</commit_message>
<xml_diff>
--- a/variacion.xlsx
+++ b/variacion.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fecha</t>
   </si>
@@ -27,22 +27,32 @@
     <t>ibc</t>
   </si>
   <si>
-    <t>var2</t>
-  </si>
-  <si>
     <t>usd</t>
   </si>
   <si>
+    <t>btc</t>
+  </si>
+  <si>
+    <t>varbtc</t>
+  </si>
+  <si>
     <t>inflacion</t>
+  </si>
+  <si>
+    <t>varusd</t>
+  </si>
+  <si>
+    <t>varibc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="mm\-yyyy"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -522,7 +532,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -535,6 +545,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -857,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +883,7 @@
     <col min="4" max="4" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,21 +891,27 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43410</v>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>43405</v>
       </c>
       <c r="B2" s="3">
         <v>507.32</v>
@@ -910,10 +928,16 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43440</v>
+      <c r="G2">
+        <v>6400</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>43435</v>
       </c>
       <c r="B3" s="3">
         <v>822.09</v>
@@ -932,10 +956,17 @@
         <f>((E3-E2)/E2)*100</f>
         <v>119.81985738709811</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>43472</v>
+      <c r="G3">
+        <v>3800</v>
+      </c>
+      <c r="H3">
+        <f>((G3-G2)/G2)*100</f>
+        <v>-40.625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>43466</v>
       </c>
       <c r="B4" s="3">
         <v>2367.5500000000002</v>
@@ -954,10 +985,17 @@
         <f t="shared" ref="F4:F19" si="0">((E4-E3)/E3)*100</f>
         <v>72.755382718391346</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>43503</v>
+      <c r="G4">
+        <v>4050</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H19" si="1">((G4-G3)/G3)*100</f>
+        <v>6.5789473684210522</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>43497</v>
       </c>
       <c r="B5" s="3">
         <v>5699.8</v>
@@ -976,10 +1014,17 @@
         <f t="shared" si="0"/>
         <v>208.37725655554092</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>43531</v>
+      <c r="G5">
+        <v>3650</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>-9.8765432098765427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>43525</v>
       </c>
       <c r="B6" s="3">
         <v>9837.64</v>
@@ -998,16 +1043,23 @@
         <f t="shared" si="0"/>
         <v>30.815822926792784</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>43563</v>
+      <c r="G6">
+        <v>3910</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>7.1232876712328768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>43556</v>
       </c>
       <c r="B7" s="3">
         <v>8683.9599999999991</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C17" si="1">((B7-B6)/B6)*100</f>
+        <f t="shared" ref="C7:C17" si="2">((B7-B6)/B6)*100</f>
         <v>-11.727202865727964</v>
       </c>
       <c r="D7">
@@ -1020,16 +1072,23 @@
         <f t="shared" si="0"/>
         <v>3.413415211746071</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>43593</v>
+      <c r="G7">
+        <v>5235</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>33.887468030690535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>43586</v>
       </c>
       <c r="B8" s="3">
         <v>15277.27</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75.925153962017362</v>
       </c>
       <c r="D8">
@@ -1042,16 +1101,23 @@
         <f t="shared" si="0"/>
         <v>54.93374816405818</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>43626</v>
+      <c r="G8">
+        <v>5850</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>11.74785100286533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>43617</v>
       </c>
       <c r="B9" s="3">
         <v>13571.37</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-11.166262035036361</v>
       </c>
       <c r="D9">
@@ -1064,16 +1130,23 @@
         <f t="shared" si="0"/>
         <v>7.8504625264391867</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>43655</v>
+      <c r="G9">
+        <v>7600</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>29.914529914529915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>43647</v>
       </c>
       <c r="B10" s="3">
         <v>19516.099999999999</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>43.80346273073387</v>
       </c>
       <c r="D10">
@@ -1086,16 +1159,23 @@
         <f t="shared" si="0"/>
         <v>22.788520912882941</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>43686</v>
+      <c r="G10">
+        <v>12950</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>70.39473684210526</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>43678</v>
       </c>
       <c r="B11" s="3">
         <v>40439.29</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>107.20989337008933</v>
       </c>
       <c r="D11">
@@ -1108,16 +1188,23 @@
         <f t="shared" si="0"/>
         <v>77.135079173460639</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>43718</v>
+      <c r="G11">
+        <v>11600</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>-10.424710424710424</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>43709</v>
       </c>
       <c r="B12" s="3">
         <v>61085.03</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51.053665877912294</v>
       </c>
       <c r="D12">
@@ -1130,16 +1217,23 @@
         <f t="shared" si="0"/>
         <v>59.594264574666546</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>43747</v>
+      <c r="G12">
+        <v>10390</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>-10.431034482758621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>43739</v>
       </c>
       <c r="B13" s="3">
         <v>52777.46</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-13.600009691408843</v>
       </c>
       <c r="D13">
@@ -1152,16 +1246,23 @@
         <f t="shared" si="0"/>
         <v>-9.1680390415506121</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>43780</v>
+      <c r="G13">
+        <v>8200</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>-21.07795957651588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>43770</v>
       </c>
       <c r="B14" s="3">
         <v>57077.23</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1469816849844694</v>
       </c>
       <c r="D14">
@@ -1174,16 +1275,23 @@
         <f t="shared" si="0"/>
         <v>45.046948051883163</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>43810</v>
+      <c r="G14">
+        <v>9240</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>12.682926829268293</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>43800</v>
       </c>
       <c r="B15" s="3">
         <v>61917.54</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4802818917456175</v>
       </c>
       <c r="D15">
@@ -1196,16 +1304,23 @@
         <f t="shared" si="0"/>
         <v>61.331754857189701</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>43843</v>
+      <c r="G15">
+        <v>7270</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>-21.320346320346321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>43831</v>
       </c>
       <c r="B16" s="4">
         <v>123483.57</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.432293337235294</v>
       </c>
       <c r="D16">
@@ -1218,16 +1333,23 @@
         <f t="shared" si="0"/>
         <v>72.342099470538884</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>43875</v>
+      <c r="G16">
+        <v>8270</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>13.75515818431912</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>43862</v>
       </c>
       <c r="B17" s="5">
         <v>123888.89</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.32823799959783506</v>
       </c>
       <c r="D17">
@@ -1240,10 +1362,17 @@
         <f t="shared" si="0"/>
         <v>-6.7513384220791544</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>43903</v>
+      <c r="G17">
+        <v>9780</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>18.258766626360341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>43891</v>
       </c>
       <c r="B18" s="3">
         <v>105807.64</v>
@@ -1262,10 +1391,17 @@
         <f t="shared" si="0"/>
         <v>6.3118597313134863</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>43929</v>
+      <c r="G18">
+        <v>4500</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>-53.987730061349694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>43922</v>
       </c>
       <c r="B19" s="3">
         <v>191984.67</v>
@@ -1281,6 +1417,13 @@
       <c r="F19">
         <f t="shared" si="0"/>
         <v>46.701268307507917</v>
+      </c>
+      <c r="G19">
+        <v>7250</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>61.111111111111114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>